<commit_message>
CGC : Tax Logic Fixes
</commit_message>
<xml_diff>
--- a/capital_gain_calculator/Dashboards/Dashboardv3.xlsx
+++ b/capital_gain_calculator/Dashboards/Dashboardv3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITR-Kit\short_sale_calculator\Dashboards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITR-Kit\capital_gain_calculator\Dashboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C526A42-5234-49B3-9FBF-DE6A8E33ADBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5D0C8D-D86A-4515-8A03-33B03AB149FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{84E4215D-59A1-47B3-B7C6-EBA92DED9849}"/>
   </bookViews>
@@ -257,40 +257,40 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -639,8 +639,8 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:E11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.140625" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -651,13 +651,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
@@ -669,47 +669,47 @@
       <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="13"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="6">
-        <v>50000</v>
+        <v>80000</v>
       </c>
       <c r="C3" s="6">
-        <v>40000</v>
+        <v>75000</v>
       </c>
       <c r="D3" s="6">
-        <f>ROUND((B3-C3)*15%,0)</f>
-        <v>1500</v>
-      </c>
-      <c r="E3" s="18">
+        <f>IF(B3-C3&gt;=0,ROUND((B3-C3)*15%,0),0)</f>
+        <v>750</v>
+      </c>
+      <c r="E3" s="12">
         <f>D3+D4</f>
-        <v>500</v>
-      </c>
-      <c r="F3" s="14"/>
+        <v>750</v>
+      </c>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="6">
-        <v>5000</v>
+        <v>80000</v>
       </c>
       <c r="C4" s="6">
-        <v>10000</v>
+        <v>90000</v>
       </c>
       <c r="D4" s="6">
-        <f>ROUND((B4-C4)*20%,0)</f>
-        <v>-1000</v>
-      </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="14"/>
+        <f>IF(B4-C4&gt;=0,ROUND((B4-C4)*20%,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -717,27 +717,27 @@
       </c>
       <c r="B5" s="9">
         <f>B3+B4</f>
-        <v>55000</v>
+        <v>160000</v>
       </c>
       <c r="C5" s="9">
         <f>C3+C4</f>
-        <v>50000</v>
+        <v>165000</v>
       </c>
       <c r="D5" s="9">
         <f>D3+D4</f>
-        <v>500</v>
-      </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="14"/>
+        <v>750</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -749,10 +749,10 @@
       <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="17"/>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -768,28 +768,28 @@
         <f>IF(B8-C8&gt;100000,ROUND(((B8-C8)-100000)*10%,0),0)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="12">
         <f>D8+D9</f>
-        <v>19</v>
-      </c>
-      <c r="F8" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="6">
-        <v>555</v>
+        <v>300000</v>
       </c>
       <c r="C9" s="6">
-        <v>400</v>
+        <v>500000</v>
       </c>
       <c r="D9" s="6">
-        <f>ROUND((B9-C9)*12.5%,0)</f>
-        <v>19</v>
-      </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="14"/>
+        <f>IF(B9-C9&gt;125000,ROUND(((B9-C9)-125000)*12.5%,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -797,49 +797,49 @@
       </c>
       <c r="B10" s="2">
         <f>B8+B9</f>
-        <v>150555</v>
+        <v>450000</v>
       </c>
       <c r="C10" s="2">
         <f>C8+C9</f>
-        <v>300400</v>
+        <v>800000</v>
       </c>
       <c r="D10" s="2">
         <f>D8+D9</f>
-        <v>19</v>
-      </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="14">
+      <c r="B11" s="19"/>
+      <c r="C11" s="13">
         <f>SUM(E3,E8)</f>
-        <v>519</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="20"/>
+        <v>750</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="12">
         <f>B5-C5</f>
-        <v>5000</v>
-      </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="19" t="s">
+        <v>-5000</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="12">
         <f>B10-C10</f>
-        <v>-149845</v>
-      </c>
-      <c r="F12" s="14"/>
+        <v>-350000</v>
+      </c>
+      <c r="F12" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>